<commit_message>
Fixed folder names to reflect csproj titles.
</commit_message>
<xml_diff>
--- a/Design Documentation/SnapperCodingChallenge V1.1 To Do List.xlsx
+++ b/Design Documentation/SnapperCodingChallenge V1.1 To Do List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcox\Desktop\git\SnapperCodingChallenge\Design Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CD288E-8B46-4254-B43A-3463F89ED45C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F2A2FC-1EEF-45BC-B023-F4D081F87686}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>SnapperCodingChallenge V1.1 To Do List</t>
   </si>
@@ -92,6 +92,27 @@
   </si>
   <si>
     <t>Load SnaperImage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pause the Console to Allow User to Eamine Data </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summarise TargetsFound </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write Output File </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actors </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI - Something to echo whats actually going on </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dump - Something to dump whats being echoed to </t>
   </si>
 </sst>
 </file>
@@ -299,16 +320,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>561295</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>18786</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>513670</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>28311</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -331,7 +352,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2438400" y="571500"/>
+          <a:off x="4219575" y="200025"/>
           <a:ext cx="5438095" cy="2114286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -343,16 +364,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>161926</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>89996</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>13796</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -375,7 +396,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2438400" y="2828926"/>
+          <a:off x="4200525" y="2371726"/>
           <a:ext cx="5457825" cy="690070"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -687,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Z18"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC44" sqref="AC44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,37 +927,70 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F8EB1D-FA74-4494-B33B-81E41E108845}">
-  <dimension ref="B2:B25"/>
+  <dimension ref="B2:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="R6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>